<commit_message>
release: Versão final do projeto
</commit_message>
<xml_diff>
--- a/data/relatorioAbandono.xlsx
+++ b/data/relatorioAbandono.xlsx
@@ -475,19 +475,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -500,19 +500,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>